<commit_message>
3 seasons 30 levels
</commit_message>
<xml_diff>
--- a/Assets/ScriptableObjects/Marble5 levels.xlsx
+++ b/Assets/ScriptableObjects/Marble5 levels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Manu\Marble5\Assets\ScriptableObjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDA294A-A9D9-45B5-825A-A6F6B2D86415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78D10E1-7878-484C-A109-88BA21627694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{FCC4B52F-2733-4863-A5E0-8FC58FD924E4}"/>
+    <workbookView xWindow="-18285" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{FCC4B52F-2733-4863-A5E0-8FC58FD924E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -111,21 +111,6 @@
     <t>SpaceBG_10</t>
   </si>
   <si>
-    <t>SpaceBG_11</t>
-  </si>
-  <si>
-    <t>SpaceBG_12</t>
-  </si>
-  <si>
-    <t>SpaceBG_13</t>
-  </si>
-  <si>
-    <t>SpaceBG_14</t>
-  </si>
-  <si>
-    <t>SpaceBG_15</t>
-  </si>
-  <si>
     <t>BG</t>
   </si>
   <si>
@@ -150,39 +135,6 @@
     <t>Progression</t>
   </si>
   <si>
-    <t>SpaceBG_16</t>
-  </si>
-  <si>
-    <t>SpaceBG_17</t>
-  </si>
-  <si>
-    <t>SpaceBG_18</t>
-  </si>
-  <si>
-    <t>SpaceBG_19</t>
-  </si>
-  <si>
-    <t>SpaceBG_20</t>
-  </si>
-  <si>
-    <t>SpaceBG_21</t>
-  </si>
-  <si>
-    <t>SpaceBG_22</t>
-  </si>
-  <si>
-    <t>SpaceBG_23</t>
-  </si>
-  <si>
-    <t>SpaceBG_24</t>
-  </si>
-  <si>
-    <t>SpaceBG_25</t>
-  </si>
-  <si>
-    <t>SpaceBG_26</t>
-  </si>
-  <si>
     <t>Element 15</t>
   </si>
   <si>
@@ -228,16 +180,64 @@
     <t>Element 29</t>
   </si>
   <si>
-    <t>SpaceBG_27</t>
-  </si>
-  <si>
-    <t>SpaceBG_28</t>
-  </si>
-  <si>
-    <t>SpaceBG_29</t>
-  </si>
-  <si>
-    <t>SpaceBG_30</t>
+    <t>ForestBG_01</t>
+  </si>
+  <si>
+    <t>ForestBG_02</t>
+  </si>
+  <si>
+    <t>ForestBG_03</t>
+  </si>
+  <si>
+    <t>ForestBG_04</t>
+  </si>
+  <si>
+    <t>ForestBG_05</t>
+  </si>
+  <si>
+    <t>ForestBG_06</t>
+  </si>
+  <si>
+    <t>ForestBG_07</t>
+  </si>
+  <si>
+    <t>ForestBG_08</t>
+  </si>
+  <si>
+    <t>ForestBG_09</t>
+  </si>
+  <si>
+    <t>ForestBG_10</t>
+  </si>
+  <si>
+    <t>RuinsBG_01</t>
+  </si>
+  <si>
+    <t>RuinsBG_02</t>
+  </si>
+  <si>
+    <t>RuinsBG_03</t>
+  </si>
+  <si>
+    <t>RuinsBG_04</t>
+  </si>
+  <si>
+    <t>RuinsBG_05</t>
+  </si>
+  <si>
+    <t>RuinsBG_06</t>
+  </si>
+  <si>
+    <t>RuinsBG_07</t>
+  </si>
+  <si>
+    <t>RuinsBG_08</t>
+  </si>
+  <si>
+    <t>RuinsBG_09</t>
+  </si>
+  <si>
+    <t>RuinsBG_10</t>
   </si>
 </sst>
 </file>
@@ -274,12 +274,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -287,6 +281,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,10 +310,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,16 +355,16 @@
     <tableColumn id="2" xr3:uid="{83E9CFDE-11AB-4421-BF3C-539FEA4950F2}" name="BG"/>
     <tableColumn id="3" xr3:uid="{CFF445D2-C2A2-47BC-B33B-84BF1C6D8B00}" name="Handicap"/>
     <tableColumn id="4" xr3:uid="{6F285335-3565-4E09-97BD-62F7124CD60F}" name="Difficulte"/>
-    <tableColumn id="5" xr3:uid="{7B819317-2628-407A-967E-60790634A851}" name="Star 1" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{7B819317-2628-407A-967E-60790634A851}" name="Star 1" dataDxfId="2">
       <calculatedColumnFormula>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7F140BCF-AB83-4A28-8C16-CCE4E0CBFDB9}" name="Star 2" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{7F140BCF-AB83-4A28-8C16-CCE4E0CBFDB9}" name="Star 2" dataDxfId="1">
       <calculatedColumnFormula>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{017DE0A1-AEDF-41C0-9774-EA424BE59870}" name="Star 3">
       <calculatedColumnFormula>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C492EF36-1AD0-4EC7-AA3B-0F88A02D6994}" name="Progression" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{C492EF36-1AD0-4EC7-AA3B-0F88A02D6994}" name="Progression" dataDxfId="0">
       <calculatedColumnFormula>D4*2+(6-E4)*2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -671,59 +671,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A73136-3146-4EA3-B08F-5FC9620F39B9}">
   <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="9" width="16.26953125" customWidth="1"/>
+    <col min="2" max="9" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F2" s="5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="4">
         <v>2</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>1.5</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -747,13 +747,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -777,13 +777,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -807,13 +807,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -837,13 +837,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -867,13 +867,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -897,13 +897,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -927,13 +927,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -958,13 +958,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -989,13 +989,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -1020,13 +1020,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1051,13 +1051,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -1082,13 +1082,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1113,13 +1113,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -1144,13 +1144,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1175,13 +1175,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1206,13 +1206,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D20">
         <v>6</v>
@@ -1237,13 +1237,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -1268,13 +1268,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1299,13 +1299,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -1330,13 +1330,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1361,13 +1361,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1392,13 +1392,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D26">
         <v>6</v>
@@ -1423,13 +1423,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -1454,13 +1454,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -1485,13 +1485,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D29">
         <v>5</v>
@@ -1516,13 +1516,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1547,13 +1547,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="D31">
         <v>6</v>
@@ -1578,13 +1578,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="4"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="D32">
         <v>4</v>
@@ -1609,13 +1609,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="4"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="D33">
         <v>5</v>

</xml_diff>

<commit_message>
First star levels + ranking
</commit_message>
<xml_diff>
--- a/Assets/ScriptableObjects/Marble5 levels.xlsx
+++ b/Assets/ScriptableObjects/Marble5 levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Manu\Marble5\Assets\ScriptableObjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78D10E1-7878-484C-A109-88BA21627694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE3899E-844B-4363-877A-32CA80ED38CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18285" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{FCC4B52F-2733-4863-A5E0-8FC58FD924E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{FCC4B52F-2733-4863-A5E0-8FC58FD924E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -355,16 +355,16 @@
     <tableColumn id="2" xr3:uid="{83E9CFDE-11AB-4421-BF3C-539FEA4950F2}" name="BG"/>
     <tableColumn id="3" xr3:uid="{CFF445D2-C2A2-47BC-B33B-84BF1C6D8B00}" name="Handicap"/>
     <tableColumn id="4" xr3:uid="{6F285335-3565-4E09-97BD-62F7124CD60F}" name="Difficulte"/>
-    <tableColumn id="5" xr3:uid="{7B819317-2628-407A-967E-60790634A851}" name="Star 1" dataDxfId="2">
-      <calculatedColumnFormula>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{7B819317-2628-407A-967E-60790634A851}" name="Star 1" dataDxfId="0">
+      <calculatedColumnFormula>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7F140BCF-AB83-4A28-8C16-CCE4E0CBFDB9}" name="Star 2" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{7F140BCF-AB83-4A28-8C16-CCE4E0CBFDB9}" name="Star 2" dataDxfId="2">
       <calculatedColumnFormula>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{017DE0A1-AEDF-41C0-9774-EA424BE59870}" name="Star 3">
       <calculatedColumnFormula>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C492EF36-1AD0-4EC7-AA3B-0F88A02D6994}" name="Progression" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{C492EF36-1AD0-4EC7-AA3B-0F88A02D6994}" name="Progression" dataDxfId="1">
       <calculatedColumnFormula>D4*2+(6-E4)*2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A73136-3146-4EA3-B08F-5FC9620F39B9}">
   <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,12 +732,12 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>60</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>55</v>
       </c>
       <c r="G4">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H4">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -762,12 +762,12 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>60</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>55</v>
       </c>
       <c r="G5">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H5">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -792,12 +792,12 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>59</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>54</v>
       </c>
       <c r="G6">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H6">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -822,12 +822,12 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>59</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>54</v>
       </c>
       <c r="G7">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H7">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -852,12 +852,12 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>58</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>53</v>
       </c>
       <c r="G8">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H8">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -882,12 +882,12 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>58</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>53</v>
       </c>
       <c r="G9">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H9">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -912,12 +912,12 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>57</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>52</v>
       </c>
       <c r="G10">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H10">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -942,12 +942,12 @@
         <v>5</v>
       </c>
       <c r="F11">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>53</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>48</v>
       </c>
       <c r="G11">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H11">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -973,12 +973,12 @@
         <v>5</v>
       </c>
       <c r="F12">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>51</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>46</v>
       </c>
       <c r="G12">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H12">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1004,12 +1004,12 @@
         <v>5</v>
       </c>
       <c r="F13">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>49</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>44</v>
       </c>
       <c r="G13">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H13">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1035,12 +1035,12 @@
         <v>4</v>
       </c>
       <c r="F14">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>48</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>43</v>
       </c>
       <c r="G14">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H14">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1066,12 +1066,12 @@
         <v>5</v>
       </c>
       <c r="F15">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>47</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>42</v>
       </c>
       <c r="G15">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H15">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1097,12 +1097,12 @@
         <v>4</v>
       </c>
       <c r="F16">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>46</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>41</v>
       </c>
       <c r="G16">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H16">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1128,12 +1128,12 @@
         <v>5</v>
       </c>
       <c r="F17">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>45</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>40</v>
       </c>
       <c r="G17">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H17">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1159,12 +1159,12 @@
         <v>4</v>
       </c>
       <c r="F18">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>44</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>39</v>
       </c>
       <c r="G18">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H18">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1190,12 +1190,12 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>43</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>38</v>
       </c>
       <c r="G19">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H19">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1221,12 +1221,12 @@
         <v>5</v>
       </c>
       <c r="F20">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>43</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>38</v>
       </c>
       <c r="G20">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H20">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1252,12 +1252,12 @@
         <v>4</v>
       </c>
       <c r="F21">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>42</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>37</v>
       </c>
       <c r="G21">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H21">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1283,12 +1283,12 @@
         <v>3</v>
       </c>
       <c r="F22">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>41</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>36</v>
       </c>
       <c r="G22">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H22">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1314,12 +1314,12 @@
         <v>4</v>
       </c>
       <c r="F23">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>40</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>35</v>
       </c>
       <c r="G23">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H23">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1345,12 +1345,12 @@
         <v>3</v>
       </c>
       <c r="F24">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>39</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>34</v>
       </c>
       <c r="G24">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H24">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1376,12 +1376,12 @@
         <v>2</v>
       </c>
       <c r="F25">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>38</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>33</v>
       </c>
       <c r="G25">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H25">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1407,12 +1407,12 @@
         <v>4</v>
       </c>
       <c r="F26">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>38</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>33</v>
       </c>
       <c r="G26">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H26">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1438,12 +1438,12 @@
         <v>3</v>
       </c>
       <c r="F27">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>37</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>32</v>
       </c>
       <c r="G27">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H27">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1469,12 +1469,12 @@
         <v>2</v>
       </c>
       <c r="F28">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>36</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>31</v>
       </c>
       <c r="G28">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H28">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1500,12 +1500,12 @@
         <v>3</v>
       </c>
       <c r="F29">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>35</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>30</v>
       </c>
       <c r="G29">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H29">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1531,12 +1531,12 @@
         <v>2</v>
       </c>
       <c r="F30">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>34</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>29</v>
       </c>
       <c r="G30">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H30">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1562,12 +1562,12 @@
         <v>3</v>
       </c>
       <c r="F31">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>33</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>28</v>
       </c>
       <c r="G31">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H31">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1593,12 +1593,12 @@
         <v>2</v>
       </c>
       <c r="F32">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>32</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>27</v>
       </c>
       <c r="G32">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H32">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>
@@ -1624,12 +1624,12 @@
         <v>2</v>
       </c>
       <c r="F33">
-        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)</f>
-        <v>30</v>
+        <f>ROUND(60-Tableau1[[#This Row],[Progression]]/$F$2,0)-5</f>
+        <v>25</v>
       </c>
       <c r="G33">
         <f>ROUND(AVERAGE(Tableau1[[#This Row],[Star 1]],Tableau1[[#This Row],[Star 3]]),0)</f>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H33">
         <f>ROUND(100-Tableau1[[#This Row],[Progression]]/$H$2,0)</f>

</xml_diff>